<commit_message>
switched branches to fix push/pull issue
</commit_message>
<xml_diff>
--- a/Project 2 Documentation/Burndown Chart/Burndown Chart chatapredu.xlsx
+++ b/Project 2 Documentation/Burndown Chart/Burndown Chart chatapredu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taiwo\Desktop\Revature Training\May 24th Batch\Project 2\docs\Project 2 Documentation\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44938F6C-3BD6-4CF7-A5E7-F951BDA94A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79F1C6D-FE28-44A8-BBFD-63F204527692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{278249F8-2613-4AF5-B591-A033C8328AD7}"/>
   </bookViews>
@@ -345,19 +345,19 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -540,6 +540,9 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
@@ -1000,19 +1003,19 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1195,6 +1198,9 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
@@ -2878,8 +2884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F39199-5982-4E68-B6B2-9AB0222183E4}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3092,7 +3098,7 @@
         <v>44396</v>
       </c>
       <c r="B19">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>33</v>
@@ -3103,7 +3109,10 @@
         <v>44397</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -3111,7 +3120,7 @@
         <v>44398</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -3119,7 +3128,7 @@
         <v>44399</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -3127,7 +3136,7 @@
         <v>44400</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>